<commit_message>
UserConfigurations implemented - It lack for proving that the code is functional
</commit_message>
<xml_diff>
--- a/Template/PlantillaCreacionKactus.xlsx
+++ b/Template/PlantillaCreacionKactus.xlsx
@@ -116,7 +116,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -126,6 +126,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -252,10 +256,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -273,10 +277,10 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="n">
-        <v>10198901245</v>
+        <v>1023866054</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>133</v>
+        <v>196</v>
       </c>
       <c r="C2" s="2" t="n">
         <v>3</v>
@@ -284,68 +288,101 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="n">
-        <v>1033754995</v>
+        <v>1052412499</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>101</v>
+        <v>196</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
-        <v>1010178996</v>
+      <c r="A4" s="3" t="n">
+        <v>1098658561</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>133</v>
-      </c>
-      <c r="C4" s="0" t="n">
+        <v>195</v>
+      </c>
+      <c r="C4" s="3" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
-        <v>80219752</v>
+      <c r="A5" s="3" t="n">
+        <v>63528540</v>
       </c>
       <c r="B5" s="2" t="n">
-        <v>101</v>
-      </c>
-      <c r="C5" s="0" t="n">
+        <v>195</v>
+      </c>
+      <c r="C5" s="3" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
-        <v>1001347043</v>
+      <c r="A6" s="3" t="n">
+        <v>39427884</v>
       </c>
       <c r="B6" s="2" t="n">
-        <v>133</v>
-      </c>
-      <c r="C6" s="0" t="n">
+        <v>194</v>
+      </c>
+      <c r="C6" s="3" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
-        <v>1014267333</v>
+      <c r="A7" s="3" t="n">
+        <v>1040370636</v>
       </c>
       <c r="B7" s="2" t="n">
-        <v>101</v>
-      </c>
-      <c r="C7" s="0" t="n">
+        <v>194</v>
+      </c>
+      <c r="C7" s="3" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
-        <v>1077148146</v>
-      </c>
-      <c r="B8" s="0" t="n">
-        <v>133</v>
-      </c>
-      <c r="C8" s="0" t="n">
-        <v>3</v>
+      <c r="A8" s="3" t="n">
+        <v>80125674</v>
+      </c>
+      <c r="B8" s="3" t="n">
+        <v>196</v>
+      </c>
+      <c r="C8" s="3" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>1032445017</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>196</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>1014186124</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>195</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>39424174</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>194</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bugs fixed - Dictionaries created
</commit_message>
<xml_diff>
--- a/Template/PlantillaCreacionKactus.xlsx
+++ b/Template/PlantillaCreacionKactus.xlsx
@@ -20,15 +20,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="4">
   <si>
     <t xml:space="preserve">Documento</t>
   </si>
   <si>
-    <t xml:space="preserve">Grupo</t>
+    <t xml:space="preserve">Perfil</t>
   </si>
   <si>
-    <t xml:space="preserve">Perfil</t>
+    <t xml:space="preserve">Usuario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supervisor</t>
   </si>
 </sst>
 </file>
@@ -256,10 +259,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -271,118 +274,85 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="n">
         <v>1023866054</v>
       </c>
-      <c r="B2" s="2" t="n">
-        <v>196</v>
-      </c>
-      <c r="C2" s="2" t="n">
-        <v>3</v>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="n">
         <v>1052412499</v>
       </c>
-      <c r="B3" s="2" t="n">
-        <v>196</v>
-      </c>
-      <c r="C3" s="2" t="n">
-        <v>3</v>
+      <c r="B3" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="n">
         <v>1098658561</v>
       </c>
-      <c r="B4" s="2" t="n">
-        <v>195</v>
-      </c>
-      <c r="C4" s="3" t="n">
-        <v>3</v>
+      <c r="B4" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="n">
         <v>63528540</v>
       </c>
-      <c r="B5" s="2" t="n">
-        <v>195</v>
-      </c>
-      <c r="C5" s="3" t="n">
-        <v>3</v>
+      <c r="B5" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="n">
         <v>39427884</v>
       </c>
-      <c r="B6" s="2" t="n">
-        <v>194</v>
-      </c>
-      <c r="C6" s="3" t="n">
-        <v>3</v>
+      <c r="B6" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="n">
         <v>1040370636</v>
       </c>
-      <c r="B7" s="2" t="n">
-        <v>194</v>
-      </c>
-      <c r="C7" s="3" t="n">
-        <v>3</v>
+      <c r="B7" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="n">
         <v>80125674</v>
       </c>
-      <c r="B8" s="3" t="n">
-        <v>196</v>
-      </c>
-      <c r="C8" s="3" t="n">
-        <v>4</v>
+      <c r="B8" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
+      <c r="A9" s="3" t="n">
         <v>1032445017</v>
       </c>
-      <c r="B9" s="0" t="n">
-        <v>196</v>
-      </c>
-      <c r="C9" s="0" t="n">
-        <v>4</v>
+      <c r="B9" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
+      <c r="A10" s="3" t="n">
         <v>1014186124</v>
       </c>
-      <c r="B10" s="0" t="n">
-        <v>195</v>
-      </c>
-      <c r="C10" s="0" t="n">
-        <v>4</v>
+      <c r="B10" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
+      <c r="A11" s="3" t="n">
         <v>39424174</v>
       </c>
-      <c r="B11" s="0" t="n">
-        <v>194</v>
-      </c>
-      <c r="C11" s="0" t="n">
-        <v>4</v>
+      <c r="B11" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactoring to split Supervisor and User requests - trying requests twice if needed
</commit_message>
<xml_diff>
--- a/Template/PlantillaCreacionKactus.xlsx
+++ b/Template/PlantillaCreacionKactus.xlsx
@@ -262,7 +262,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -277,15 +277,15 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="n">
-        <v>1023866054</v>
+        <v>1052412499</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="n">
-        <v>1052412499</v>
+      <c r="A3" s="3" t="n">
+        <v>63528540</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>2</v>
@@ -293,7 +293,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="n">
-        <v>1098658561</v>
+        <v>39427884</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>2</v>
@@ -301,7 +301,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="n">
-        <v>63528540</v>
+        <v>1040370636</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>2</v>
@@ -309,23 +309,23 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="n">
-        <v>39427884</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>2</v>
+        <v>80125674</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="n">
-        <v>1040370636</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>2</v>
+        <v>1014186124</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="n">
-        <v>80125674</v>
+        <v>39424174</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>3</v>
@@ -333,26 +333,26 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="n">
-        <v>1032445017</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>3</v>
+        <v>1098658561</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="n">
-        <v>1014186124</v>
+        <v>1032445017</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="n">
-        <v>39424174</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>3</v>
+      <c r="A11" s="2" t="n">
+        <v>1023866054</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>